<commit_message>
Change opcodes in hex to opcode binary vectors
Signed-off-by: JayJay <jwanjohi95@gmail.com>
</commit_message>
<xml_diff>
--- a/Java_Bytecode_Instructions.xlsx
+++ b/Java_Bytecode_Instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="411">
   <si>
     <t>aaload</t>
   </si>
@@ -41,81 +41,42 @@
     <t>aload_0</t>
   </si>
   <si>
-    <t>2a</t>
-  </si>
-  <si>
     <t>aload_1</t>
   </si>
   <si>
-    <t>2b</t>
-  </si>
-  <si>
     <t>aload_2</t>
   </si>
   <si>
-    <t>2c</t>
-  </si>
-  <si>
     <t>aload_3</t>
   </si>
   <si>
-    <t>2d</t>
-  </si>
-  <si>
     <t>anewarray</t>
   </si>
   <si>
-    <t>bd</t>
-  </si>
-  <si>
     <t>areturn</t>
   </si>
   <si>
-    <t>b0</t>
-  </si>
-  <si>
     <t>arraylength</t>
   </si>
   <si>
-    <t>be</t>
-  </si>
-  <si>
     <t>astore</t>
   </si>
   <si>
-    <t>3a</t>
-  </si>
-  <si>
     <t>astore_0</t>
   </si>
   <si>
-    <t>4b</t>
-  </si>
-  <si>
     <t>astore_1</t>
   </si>
   <si>
-    <t>4c</t>
-  </si>
-  <si>
     <t>astore_2</t>
   </si>
   <si>
-    <t>4d</t>
-  </si>
-  <si>
     <t>astore_3</t>
   </si>
   <si>
-    <t>4e</t>
-  </si>
-  <si>
     <t>athrow</t>
   </si>
   <si>
-    <t>bf</t>
-  </si>
-  <si>
     <t>baload</t>
   </si>
   <si>
@@ -128,9 +89,6 @@
     <t>breakpoint</t>
   </si>
   <si>
-    <t>ca</t>
-  </si>
-  <si>
     <t>caload</t>
   </si>
   <si>
@@ -140,24 +98,15 @@
     <t>checkcast</t>
   </si>
   <si>
-    <t>c0</t>
-  </si>
-  <si>
     <t>d2f</t>
   </si>
   <si>
     <t>d2i</t>
   </si>
   <si>
-    <t>8e</t>
-  </si>
-  <si>
     <t>d2l</t>
   </si>
   <si>
-    <t>8f</t>
-  </si>
-  <si>
     <t>dadd</t>
   </si>
   <si>
@@ -176,21 +125,12 @@
     <t>dconst_0</t>
   </si>
   <si>
-    <t>0e</t>
-  </si>
-  <si>
     <t>dconst_1</t>
   </si>
   <si>
-    <t>0f</t>
-  </si>
-  <si>
     <t>ddiv</t>
   </si>
   <si>
-    <t>6f</t>
-  </si>
-  <si>
     <t>dload</t>
   </si>
   <si>
@@ -209,9 +149,6 @@
     <t>dmul</t>
   </si>
   <si>
-    <t>6b</t>
-  </si>
-  <si>
     <t>dneg</t>
   </si>
   <si>
@@ -221,9 +158,6 @@
     <t>dreturn</t>
   </si>
   <si>
-    <t>af</t>
-  </si>
-  <si>
     <t>dstore</t>
   </si>
   <si>
@@ -239,9 +173,6 @@
     <t>dstore_3</t>
   </si>
   <si>
-    <t>4a</t>
-  </si>
-  <si>
     <t>dsub</t>
   </si>
   <si>
@@ -251,51 +182,27 @@
     <t>dup_x1</t>
   </si>
   <si>
-    <t>5a</t>
-  </si>
-  <si>
     <t>dup_x2</t>
   </si>
   <si>
-    <t>5b</t>
-  </si>
-  <si>
     <t>dup2</t>
   </si>
   <si>
-    <t>5c</t>
-  </si>
-  <si>
     <t>dup2_x1</t>
   </si>
   <si>
-    <t>5d</t>
-  </si>
-  <si>
     <t>dup2_x2</t>
   </si>
   <si>
-    <t>5e</t>
-  </si>
-  <si>
     <t>f2d</t>
   </si>
   <si>
-    <t>8d</t>
-  </si>
-  <si>
     <t>f2i</t>
   </si>
   <si>
-    <t>8b</t>
-  </si>
-  <si>
     <t>f2l</t>
   </si>
   <si>
-    <t>8c</t>
-  </si>
-  <si>
     <t>fadd</t>
   </si>
   <si>
@@ -314,27 +221,15 @@
     <t>fconst_0</t>
   </si>
   <si>
-    <t>0b</t>
-  </si>
-  <si>
     <t>fconst_1</t>
   </si>
   <si>
-    <t>0c</t>
-  </si>
-  <si>
     <t>fconst_2</t>
   </si>
   <si>
-    <t>0d</t>
-  </si>
-  <si>
     <t>fdiv</t>
   </si>
   <si>
-    <t>6e</t>
-  </si>
-  <si>
     <t>fload</t>
   </si>
   <si>
@@ -353,9 +248,6 @@
     <t>fmul</t>
   </si>
   <si>
-    <t>6a</t>
-  </si>
-  <si>
     <t>fneg</t>
   </si>
   <si>
@@ -365,9 +257,6 @@
     <t>freturn</t>
   </si>
   <si>
-    <t>ae</t>
-  </si>
-  <si>
     <t>fstore</t>
   </si>
   <si>
@@ -389,27 +278,15 @@
     <t>getfield</t>
   </si>
   <si>
-    <t>b4</t>
-  </si>
-  <si>
     <t>getstatic</t>
   </si>
   <si>
-    <t>b2</t>
-  </si>
-  <si>
     <t>goto</t>
   </si>
   <si>
-    <t>a7</t>
-  </si>
-  <si>
     <t>goto_w</t>
   </si>
   <si>
-    <t>c8</t>
-  </si>
-  <si>
     <t>i2b</t>
   </si>
   <si>
@@ -434,21 +311,12 @@
     <t>iaload</t>
   </si>
   <si>
-    <t>2e</t>
-  </si>
-  <si>
     <t>iand</t>
   </si>
   <si>
-    <t>7e</t>
-  </si>
-  <si>
     <t>iastore</t>
   </si>
   <si>
-    <t>4f</t>
-  </si>
-  <si>
     <t>iconst_m1</t>
   </si>
   <si>
@@ -473,102 +341,54 @@
     <t>idiv</t>
   </si>
   <si>
-    <t>6c</t>
-  </si>
-  <si>
     <t>if_acmpeq</t>
   </si>
   <si>
-    <t>a5</t>
-  </si>
-  <si>
     <t>if_acmpne</t>
   </si>
   <si>
-    <t>a6</t>
-  </si>
-  <si>
     <t>if_icmpeq</t>
   </si>
   <si>
-    <t>9f</t>
-  </si>
-  <si>
     <t>if_icmpge</t>
   </si>
   <si>
-    <t>a2</t>
-  </si>
-  <si>
     <t>if_icmpgt</t>
   </si>
   <si>
-    <t>a3</t>
-  </si>
-  <si>
     <t>if_icmple</t>
   </si>
   <si>
-    <t>a4</t>
-  </si>
-  <si>
     <t>if_icmplt</t>
   </si>
   <si>
-    <t>a1</t>
-  </si>
-  <si>
     <t>if_icmpne</t>
   </si>
   <si>
-    <t>a0</t>
-  </si>
-  <si>
     <t>ifeq</t>
   </si>
   <si>
     <t>ifge</t>
   </si>
   <si>
-    <t>9c</t>
-  </si>
-  <si>
     <t>ifgt</t>
   </si>
   <si>
-    <t>9d</t>
-  </si>
-  <si>
     <t>ifle</t>
   </si>
   <si>
-    <t>9e</t>
-  </si>
-  <si>
     <t>iflt</t>
   </si>
   <si>
-    <t>9b</t>
-  </si>
-  <si>
     <t>ifne</t>
   </si>
   <si>
-    <t>9a</t>
-  </si>
-  <si>
     <t>ifnonnull</t>
   </si>
   <si>
-    <t>c7</t>
-  </si>
-  <si>
     <t>ifnull</t>
   </si>
   <si>
-    <t>c6</t>
-  </si>
-  <si>
     <t>iinc</t>
   </si>
   <si>
@@ -578,39 +398,21 @@
     <t>iload_0</t>
   </si>
   <si>
-    <t>1a</t>
-  </si>
-  <si>
     <t>iload_1</t>
   </si>
   <si>
-    <t>1b</t>
-  </si>
-  <si>
     <t>iload_2</t>
   </si>
   <si>
-    <t>1c</t>
-  </si>
-  <si>
     <t>iload_3</t>
   </si>
   <si>
-    <t>1d</t>
-  </si>
-  <si>
     <t>impdep1</t>
   </si>
   <si>
-    <t>fe</t>
-  </si>
-  <si>
     <t>impdep2</t>
   </si>
   <si>
-    <t>ff</t>
-  </si>
-  <si>
     <t>imul</t>
   </si>
   <si>
@@ -620,39 +422,21 @@
     <t>instanceof</t>
   </si>
   <si>
-    <t>c1</t>
-  </si>
-  <si>
     <t>invokedynamic</t>
   </si>
   <si>
-    <t>ba</t>
-  </si>
-  <si>
     <t>invokeinterface</t>
   </si>
   <si>
-    <t>b9</t>
-  </si>
-  <si>
     <t>invokespecial</t>
   </si>
   <si>
-    <t>b7</t>
-  </si>
-  <si>
     <t>invokestatic</t>
   </si>
   <si>
-    <t>b8</t>
-  </si>
-  <si>
     <t>invokevirtual</t>
   </si>
   <si>
-    <t>b6</t>
-  </si>
-  <si>
     <t>ior</t>
   </si>
   <si>
@@ -662,75 +446,45 @@
     <t>ireturn</t>
   </si>
   <si>
-    <t>ac</t>
-  </si>
-  <si>
     <t>ishl</t>
   </si>
   <si>
     <t>ishr</t>
   </si>
   <si>
-    <t>7a</t>
-  </si>
-  <si>
     <t>istore</t>
   </si>
   <si>
     <t>istore_0</t>
   </si>
   <si>
-    <t>3b</t>
-  </si>
-  <si>
     <t>istore_1</t>
   </si>
   <si>
-    <t>3c</t>
-  </si>
-  <si>
     <t>istore_2</t>
   </si>
   <si>
-    <t>3d</t>
-  </si>
-  <si>
     <t>istore_3</t>
   </si>
   <si>
-    <t>3e</t>
-  </si>
-  <si>
     <t>isub</t>
   </si>
   <si>
     <t>iushr</t>
   </si>
   <si>
-    <t>7c</t>
-  </si>
-  <si>
     <t>ixor</t>
   </si>
   <si>
     <t>jsr</t>
   </si>
   <si>
-    <t>a8</t>
-  </si>
-  <si>
     <t>jsr_w</t>
   </si>
   <si>
-    <t>c9</t>
-  </si>
-  <si>
     <t>l2d</t>
   </si>
   <si>
-    <t>8a</t>
-  </si>
-  <si>
     <t>l2f</t>
   </si>
   <si>
@@ -743,15 +497,9 @@
     <t>laload</t>
   </si>
   <si>
-    <t>2f</t>
-  </si>
-  <si>
     <t>land</t>
   </si>
   <si>
-    <t>7f</t>
-  </si>
-  <si>
     <t>lastore</t>
   </si>
   <si>
@@ -764,9 +512,6 @@
     <t>lconst_1</t>
   </si>
   <si>
-    <t>0a</t>
-  </si>
-  <si>
     <t>ldc</t>
   </si>
   <si>
@@ -779,24 +524,15 @@
     <t>ldiv</t>
   </si>
   <si>
-    <t>6d</t>
-  </si>
-  <si>
     <t>lload</t>
   </si>
   <si>
     <t>lload_0</t>
   </si>
   <si>
-    <t>1e</t>
-  </si>
-  <si>
     <t>lload_1</t>
   </si>
   <si>
-    <t>1f</t>
-  </si>
-  <si>
     <t>lload_2</t>
   </si>
   <si>
@@ -812,9 +548,6 @@
     <t>lookupswitch</t>
   </si>
   <si>
-    <t>ab</t>
-  </si>
-  <si>
     <t>lor</t>
   </si>
   <si>
@@ -824,27 +557,18 @@
     <t>lreturn</t>
   </si>
   <si>
-    <t>ad</t>
-  </si>
-  <si>
     <t>lshl</t>
   </si>
   <si>
     <t>lshr</t>
   </si>
   <si>
-    <t>7b</t>
-  </si>
-  <si>
     <t>lstore</t>
   </si>
   <si>
     <t>lstore_0</t>
   </si>
   <si>
-    <t>3f</t>
-  </si>
-  <si>
     <t>lstore_1</t>
   </si>
   <si>
@@ -860,42 +584,24 @@
     <t>lushr</t>
   </si>
   <si>
-    <t>7d</t>
-  </si>
-  <si>
     <t>lxor</t>
   </si>
   <si>
     <t>monitorenter</t>
   </si>
   <si>
-    <t>c2</t>
-  </si>
-  <si>
     <t>monitorexit</t>
   </si>
   <si>
-    <t>c3</t>
-  </si>
-  <si>
     <t>multianewarray</t>
   </si>
   <si>
-    <t>c5</t>
-  </si>
-  <si>
     <t>new</t>
   </si>
   <si>
-    <t>bb</t>
-  </si>
-  <si>
     <t>newarray</t>
   </si>
   <si>
-    <t>bc</t>
-  </si>
-  <si>
     <t>nop</t>
   </si>
   <si>
@@ -908,27 +614,15 @@
     <t>putfield</t>
   </si>
   <si>
-    <t>b5</t>
-  </si>
-  <si>
     <t>putstatic</t>
   </si>
   <si>
-    <t>b3</t>
-  </si>
-  <si>
     <t>ret</t>
   </si>
   <si>
-    <t>a9</t>
-  </si>
-  <si>
     <t>return</t>
   </si>
   <si>
-    <t>b1</t>
-  </si>
-  <si>
     <t>saload</t>
   </si>
   <si>
@@ -941,25 +635,628 @@
     <t>swap</t>
   </si>
   <si>
-    <t>5f</t>
-  </si>
-  <si>
     <t>tableswitch</t>
   </si>
   <si>
-    <t>aa</t>
-  </si>
-  <si>
     <t>wide</t>
   </si>
   <si>
-    <t>c4</t>
-  </si>
-  <si>
     <t>(no name)</t>
   </si>
   <si>
-    <t>cb-fd</t>
+    <t>1111 1111</t>
+  </si>
+  <si>
+    <t>1111 1110</t>
+  </si>
+  <si>
+    <t>1100 1010</t>
+  </si>
+  <si>
+    <t>1100 1001</t>
+  </si>
+  <si>
+    <t>1100 1000</t>
+  </si>
+  <si>
+    <t>1100 0111</t>
+  </si>
+  <si>
+    <t>1100 0110</t>
+  </si>
+  <si>
+    <t>1100 0101</t>
+  </si>
+  <si>
+    <t>1100 0100</t>
+  </si>
+  <si>
+    <t>1100 0011</t>
+  </si>
+  <si>
+    <t>1100 0010</t>
+  </si>
+  <si>
+    <t>1100 0001</t>
+  </si>
+  <si>
+    <t>1100 0000</t>
+  </si>
+  <si>
+    <t>1011 1111</t>
+  </si>
+  <si>
+    <t>1011 1110</t>
+  </si>
+  <si>
+    <t>1011 1101</t>
+  </si>
+  <si>
+    <t>1011 1100</t>
+  </si>
+  <si>
+    <t>1011 1011</t>
+  </si>
+  <si>
+    <t>1011 1010</t>
+  </si>
+  <si>
+    <t>1011 1001</t>
+  </si>
+  <si>
+    <t>1011 1000</t>
+  </si>
+  <si>
+    <t>1011 0111</t>
+  </si>
+  <si>
+    <t>1011 0110</t>
+  </si>
+  <si>
+    <t>1011 0101</t>
+  </si>
+  <si>
+    <t>1011 0100</t>
+  </si>
+  <si>
+    <t>1011 0011</t>
+  </si>
+  <si>
+    <t>1011 0010</t>
+  </si>
+  <si>
+    <t>1011 0001</t>
+  </si>
+  <si>
+    <t>1011 0000</t>
+  </si>
+  <si>
+    <t>1010 1111</t>
+  </si>
+  <si>
+    <t>1010 1110</t>
+  </si>
+  <si>
+    <t>1010 1101</t>
+  </si>
+  <si>
+    <t>1010 1100</t>
+  </si>
+  <si>
+    <t>1010 1011</t>
+  </si>
+  <si>
+    <t>1010 1010</t>
+  </si>
+  <si>
+    <t>1010 1001</t>
+  </si>
+  <si>
+    <t>1010 1000</t>
+  </si>
+  <si>
+    <t>1010 0111</t>
+  </si>
+  <si>
+    <t>1010 0110</t>
+  </si>
+  <si>
+    <t>1010 0101</t>
+  </si>
+  <si>
+    <t>1010 0100</t>
+  </si>
+  <si>
+    <t>1010 0011</t>
+  </si>
+  <si>
+    <t>1010 0010</t>
+  </si>
+  <si>
+    <t>1010 0001</t>
+  </si>
+  <si>
+    <t>1010 0000</t>
+  </si>
+  <si>
+    <t>1001 1111</t>
+  </si>
+  <si>
+    <t>1001 1110</t>
+  </si>
+  <si>
+    <t>1001 1101</t>
+  </si>
+  <si>
+    <t>1001 1100</t>
+  </si>
+  <si>
+    <t>1001 1011</t>
+  </si>
+  <si>
+    <t>1001 1010</t>
+  </si>
+  <si>
+    <t>1001 1001</t>
+  </si>
+  <si>
+    <t>1001 1000</t>
+  </si>
+  <si>
+    <t>1001 0111</t>
+  </si>
+  <si>
+    <t>1001 0110</t>
+  </si>
+  <si>
+    <t>1001 0101</t>
+  </si>
+  <si>
+    <t>1001 0100</t>
+  </si>
+  <si>
+    <t>1001 0011</t>
+  </si>
+  <si>
+    <t>1001 0010</t>
+  </si>
+  <si>
+    <t>1001 0001</t>
+  </si>
+  <si>
+    <t>1001 0000</t>
+  </si>
+  <si>
+    <t>1000 1111</t>
+  </si>
+  <si>
+    <t>1000 1110</t>
+  </si>
+  <si>
+    <t>1000 1101</t>
+  </si>
+  <si>
+    <t>1000 1100</t>
+  </si>
+  <si>
+    <t>1000 1011</t>
+  </si>
+  <si>
+    <t>1000 1010</t>
+  </si>
+  <si>
+    <t>1000 1001</t>
+  </si>
+  <si>
+    <t>1000 1000</t>
+  </si>
+  <si>
+    <t>1000 0111</t>
+  </si>
+  <si>
+    <t>1000 0110</t>
+  </si>
+  <si>
+    <t>1000 0101</t>
+  </si>
+  <si>
+    <t>1000 0100</t>
+  </si>
+  <si>
+    <t>1000 0011</t>
+  </si>
+  <si>
+    <t>1000 0010</t>
+  </si>
+  <si>
+    <t>1000 0001</t>
+  </si>
+  <si>
+    <t>1000 0000</t>
+  </si>
+  <si>
+    <t>0111 1111</t>
+  </si>
+  <si>
+    <t>0111 1110</t>
+  </si>
+  <si>
+    <t>0111 1101</t>
+  </si>
+  <si>
+    <t>0111 1100</t>
+  </si>
+  <si>
+    <t>0111 1011</t>
+  </si>
+  <si>
+    <t>0111 1010</t>
+  </si>
+  <si>
+    <t>0111 1001</t>
+  </si>
+  <si>
+    <t>0111 1000</t>
+  </si>
+  <si>
+    <t>0111 0111</t>
+  </si>
+  <si>
+    <t>0111 0110</t>
+  </si>
+  <si>
+    <t>0111 0101</t>
+  </si>
+  <si>
+    <t>0111 0100</t>
+  </si>
+  <si>
+    <t>0111 0011</t>
+  </si>
+  <si>
+    <t>0111 0010</t>
+  </si>
+  <si>
+    <t>0111 0001</t>
+  </si>
+  <si>
+    <t>0111 0000</t>
+  </si>
+  <si>
+    <t>0110 1111</t>
+  </si>
+  <si>
+    <t>0110 1110</t>
+  </si>
+  <si>
+    <t>0110 1101</t>
+  </si>
+  <si>
+    <t>0110 1100</t>
+  </si>
+  <si>
+    <t>0110 1011</t>
+  </si>
+  <si>
+    <t>0110 1010</t>
+  </si>
+  <si>
+    <t>0110 1001</t>
+  </si>
+  <si>
+    <t>0110 1000</t>
+  </si>
+  <si>
+    <t>0110 0111</t>
+  </si>
+  <si>
+    <t>0110 0110</t>
+  </si>
+  <si>
+    <t>0110 0101</t>
+  </si>
+  <si>
+    <t>0110 0100</t>
+  </si>
+  <si>
+    <t>0110 0011</t>
+  </si>
+  <si>
+    <t>0110 0010</t>
+  </si>
+  <si>
+    <t>0110 0001</t>
+  </si>
+  <si>
+    <t>0110 0000</t>
+  </si>
+  <si>
+    <t>0101 1111</t>
+  </si>
+  <si>
+    <t>0101 1110</t>
+  </si>
+  <si>
+    <t>0101 1101</t>
+  </si>
+  <si>
+    <t>0101 1100</t>
+  </si>
+  <si>
+    <t>0101 1011</t>
+  </si>
+  <si>
+    <t>0101 1010</t>
+  </si>
+  <si>
+    <t>0101 1001</t>
+  </si>
+  <si>
+    <t>0101 1000</t>
+  </si>
+  <si>
+    <t>0101 0111</t>
+  </si>
+  <si>
+    <t>0101 0110</t>
+  </si>
+  <si>
+    <t>0101 0101</t>
+  </si>
+  <si>
+    <t>0101 0100</t>
+  </si>
+  <si>
+    <t>0101 0011</t>
+  </si>
+  <si>
+    <t>0101 0010</t>
+  </si>
+  <si>
+    <t>0101 0001</t>
+  </si>
+  <si>
+    <t>0101 0000</t>
+  </si>
+  <si>
+    <t>0100 1111</t>
+  </si>
+  <si>
+    <t>0100 1110</t>
+  </si>
+  <si>
+    <t>0100 1101</t>
+  </si>
+  <si>
+    <t>0100 1100</t>
+  </si>
+  <si>
+    <t>0100 1011</t>
+  </si>
+  <si>
+    <t>0100 1010</t>
+  </si>
+  <si>
+    <t>0100 1001</t>
+  </si>
+  <si>
+    <t>0100 1000</t>
+  </si>
+  <si>
+    <t>0100 0111</t>
+  </si>
+  <si>
+    <t>0100 0110</t>
+  </si>
+  <si>
+    <t>0100 0101</t>
+  </si>
+  <si>
+    <t>0100 0100</t>
+  </si>
+  <si>
+    <t>0100 0011</t>
+  </si>
+  <si>
+    <t>0100 0010</t>
+  </si>
+  <si>
+    <t>0100 0001</t>
+  </si>
+  <si>
+    <t>0100 0000</t>
+  </si>
+  <si>
+    <t>0011 1111</t>
+  </si>
+  <si>
+    <t>0011 1110</t>
+  </si>
+  <si>
+    <t>0011 1101</t>
+  </si>
+  <si>
+    <t>0011 1100</t>
+  </si>
+  <si>
+    <t>0011 1011</t>
+  </si>
+  <si>
+    <t>0011 1010</t>
+  </si>
+  <si>
+    <t>0011 1001</t>
+  </si>
+  <si>
+    <t>0011 1000</t>
+  </si>
+  <si>
+    <t>0011 0111</t>
+  </si>
+  <si>
+    <t>0011 0110</t>
+  </si>
+  <si>
+    <t>0011 0101</t>
+  </si>
+  <si>
+    <t>0011 0100</t>
+  </si>
+  <si>
+    <t>0011 0011</t>
+  </si>
+  <si>
+    <t>0011 0010</t>
+  </si>
+  <si>
+    <t>0011 0001</t>
+  </si>
+  <si>
+    <t>0011 0000</t>
+  </si>
+  <si>
+    <t>0010 1111</t>
+  </si>
+  <si>
+    <t>0010 1110</t>
+  </si>
+  <si>
+    <t>0010 1101</t>
+  </si>
+  <si>
+    <t>0010 1100</t>
+  </si>
+  <si>
+    <t>0010 1011</t>
+  </si>
+  <si>
+    <t>0010 1010</t>
+  </si>
+  <si>
+    <t>0010 1001</t>
+  </si>
+  <si>
+    <t>0010 1000</t>
+  </si>
+  <si>
+    <t>0010 0111</t>
+  </si>
+  <si>
+    <t>0010 0110</t>
+  </si>
+  <si>
+    <t>0010 0101</t>
+  </si>
+  <si>
+    <t>0010 0100</t>
+  </si>
+  <si>
+    <t>0010 0011</t>
+  </si>
+  <si>
+    <t>0010 0010</t>
+  </si>
+  <si>
+    <t>0010 0001</t>
+  </si>
+  <si>
+    <t>0010 0000</t>
+  </si>
+  <si>
+    <t>0001 1111</t>
+  </si>
+  <si>
+    <t>0001 1110</t>
+  </si>
+  <si>
+    <t>0001 1101</t>
+  </si>
+  <si>
+    <t>0001 1100</t>
+  </si>
+  <si>
+    <t>0001 1011</t>
+  </si>
+  <si>
+    <t>0001 1010</t>
+  </si>
+  <si>
+    <t>0001 1001</t>
+  </si>
+  <si>
+    <t>0001 1000</t>
+  </si>
+  <si>
+    <t>0001 0111</t>
+  </si>
+  <si>
+    <t>0001 0110</t>
+  </si>
+  <si>
+    <t>0001 0101</t>
+  </si>
+  <si>
+    <t>0001 0100</t>
+  </si>
+  <si>
+    <t>0001 0011</t>
+  </si>
+  <si>
+    <t>0001 0010</t>
+  </si>
+  <si>
+    <t>0001 0001</t>
+  </si>
+  <si>
+    <t>0001 0000</t>
+  </si>
+  <si>
+    <t>0000 1111</t>
+  </si>
+  <si>
+    <t>0000 1110</t>
+  </si>
+  <si>
+    <t>0000 1101</t>
+  </si>
+  <si>
+    <t>0000 1100</t>
+  </si>
+  <si>
+    <t>0000 1011</t>
+  </si>
+  <si>
+    <t>0000 1010</t>
+  </si>
+  <si>
+    <t>0000 1001</t>
+  </si>
+  <si>
+    <t>0000 1000</t>
+  </si>
+  <si>
+    <t>0000 0111</t>
+  </si>
+  <si>
+    <t>0000 0110</t>
+  </si>
+  <si>
+    <t>0000 0101</t>
+  </si>
+  <si>
+    <t>0000 0100</t>
+  </si>
+  <si>
+    <t>0000 0011</t>
+  </si>
+  <si>
+    <t>0000 0010</t>
+  </si>
+  <si>
+    <t>0000 0001</t>
+  </si>
+  <si>
+    <t>0000 0000</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1653,7 @@
   <dimension ref="A1:E206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,8 +1666,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
-        <v>32</v>
+      <c r="B1" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1380,8 +1677,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>53</v>
+      <c r="B2" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1391,8 +1688,8 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>1</v>
+      <c r="B3" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1402,8 +1699,8 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>19</v>
+      <c r="B4" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1414,7 +1711,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1422,10 +1719,10 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1433,10 +1730,10 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1444,10 +1741,10 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>213</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1455,10 +1752,10 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>214</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1466,10 +1763,10 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1477,10 +1774,10 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1488,10 +1785,10 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>217</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1499,10 +1796,10 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>218</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1510,10 +1807,10 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1521,10 +1818,10 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>25</v>
+        <v>220</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1532,10 +1829,10 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>221</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1543,10 +1840,10 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>222</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1554,10 +1851,10 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="5">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1565,10 +1862,10 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="5">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1576,10 +1873,10 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="5">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>225</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1587,10 +1884,10 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1598,10 +1895,10 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="5">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1609,10 +1906,10 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="5">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1620,10 +1917,10 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1631,10 +1928,10 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="5">
-        <v>90</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1642,10 +1939,10 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>41</v>
+        <v>231</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1653,10 +1950,10 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>232</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1664,10 +1961,10 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="5">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1675,10 +1972,10 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="5">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1686,10 +1983,10 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="5">
-        <v>52</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1697,10 +1994,10 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="5">
-        <v>98</v>
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1708,10 +2005,10 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="5">
-        <v>97</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1719,10 +2016,10 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>50</v>
+        <v>238</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1730,10 +2027,10 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>52</v>
+        <v>239</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1741,10 +2038,10 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>54</v>
+        <v>240</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1752,10 +2049,10 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="5">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1763,10 +2060,10 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="5">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1774,10 +2071,10 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="5">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1785,10 +2082,10 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="5">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1796,10 +2093,10 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="5">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>245</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1807,10 +2104,10 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>61</v>
+        <v>246</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1818,10 +2115,10 @@
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="5">
-        <v>77</v>
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1829,10 +2126,10 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="5">
-        <v>73</v>
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1840,10 +2137,10 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>65</v>
+        <v>249</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1851,10 +2148,10 @@
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="5">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1862,10 +2159,10 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="5">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1873,10 +2170,10 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" s="5">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1884,10 +2181,10 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="5">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1895,10 +2192,10 @@
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>71</v>
+        <v>254</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1906,10 +2203,10 @@
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B50" s="5">
-        <v>67</v>
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1917,10 +2214,10 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B51" s="5">
-        <v>59</v>
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1928,10 +2225,10 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>75</v>
+        <v>257</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1939,10 +2236,10 @@
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>77</v>
+        <v>258</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1950,10 +2247,10 @@
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>79</v>
+        <v>259</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1961,10 +2258,10 @@
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>81</v>
+        <v>260</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1972,10 +2269,10 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>83</v>
+        <v>261</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1983,10 +2280,10 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>85</v>
+        <v>262</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1994,10 +2291,10 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>87</v>
+        <v>263</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2005,10 +2302,10 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2016,10 +2313,10 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B60" s="5">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>265</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2027,10 +2324,10 @@
     </row>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="5">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2038,10 +2335,10 @@
     </row>
     <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B62" s="5">
-        <v>51</v>
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>267</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2049,10 +2346,10 @@
     </row>
     <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="5">
-        <v>96</v>
+        <v>62</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>268</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2060,10 +2357,10 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B64" s="5">
-        <v>95</v>
+        <v>63</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2071,10 +2368,10 @@
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>96</v>
+        <v>270</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2082,10 +2379,10 @@
     </row>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>98</v>
+        <v>271</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2093,10 +2390,10 @@
     </row>
     <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>100</v>
+        <v>272</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2104,10 +2401,10 @@
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>102</v>
+        <v>273</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2115,10 +2412,10 @@
     </row>
     <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B69" s="5">
-        <v>17</v>
+        <v>68</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2126,10 +2423,10 @@
     </row>
     <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B70" s="5">
-        <v>22</v>
+        <v>69</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>275</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2137,10 +2434,10 @@
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B71" s="5">
-        <v>23</v>
+        <v>70</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>276</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2148,10 +2445,10 @@
     </row>
     <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="5">
-        <v>24</v>
+        <v>71</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2159,10 +2456,10 @@
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B73" s="5">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>278</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2170,10 +2467,10 @@
     </row>
     <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>109</v>
+        <v>279</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2181,10 +2478,10 @@
     </row>
     <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B75" s="5">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>280</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2192,10 +2489,10 @@
     </row>
     <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B76" s="5">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>281</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2203,10 +2500,10 @@
     </row>
     <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>113</v>
+        <v>282</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2214,10 +2511,10 @@
     </row>
     <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B78" s="5">
-        <v>38</v>
+        <v>77</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2225,10 +2522,10 @@
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" s="5">
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2236,10 +2533,10 @@
     </row>
     <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B80" s="5">
-        <v>44</v>
+        <v>79</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2247,10 +2544,10 @@
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B81" s="5">
-        <v>45</v>
+        <v>80</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>286</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2258,10 +2555,10 @@
     </row>
     <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B82" s="5">
-        <v>46</v>
+        <v>81</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>287</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2269,10 +2566,10 @@
     </row>
     <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B83" s="5">
-        <v>66</v>
+        <v>82</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>288</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2280,10 +2577,10 @@
     </row>
     <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>121</v>
+        <v>289</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2291,10 +2588,10 @@
     </row>
     <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>123</v>
+        <v>290</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2302,10 +2599,10 @@
     </row>
     <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>125</v>
+        <v>291</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -2313,10 +2610,10 @@
     </row>
     <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>127</v>
+        <v>292</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -2324,10 +2621,10 @@
     </row>
     <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B88" s="5">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>293</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -2335,10 +2632,10 @@
     </row>
     <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B89" s="5">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -2346,10 +2643,10 @@
     </row>
     <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B90" s="5">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>295</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -2357,10 +2654,10 @@
     </row>
     <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B91" s="5">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>296</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -2368,10 +2665,10 @@
     </row>
     <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B92" s="5">
-        <v>85</v>
+        <v>91</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -2379,10 +2676,10 @@
     </row>
     <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B93" s="5">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>298</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -2390,10 +2687,10 @@
     </row>
     <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B94" s="5">
-        <v>60</v>
+        <v>93</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>299</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -2401,10 +2698,10 @@
     </row>
     <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>136</v>
+        <v>300</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -2412,10 +2709,10 @@
     </row>
     <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>138</v>
+        <v>301</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -2423,10 +2720,10 @@
     </row>
     <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>140</v>
+        <v>302</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -2434,10 +2731,10 @@
     </row>
     <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B98" s="5">
-        <v>2</v>
+        <v>97</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -2445,10 +2742,10 @@
     </row>
     <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B99" s="5">
-        <v>3</v>
+        <v>98</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>304</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -2456,10 +2753,10 @@
     </row>
     <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B100" s="5">
-        <v>4</v>
+        <v>99</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>305</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -2467,10 +2764,10 @@
     </row>
     <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B101" s="5">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>306</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -2478,10 +2775,10 @@
     </row>
     <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B102" s="5">
-        <v>6</v>
+        <v>101</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>307</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -2489,10 +2786,10 @@
     </row>
     <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B103" s="5">
-        <v>7</v>
+        <v>102</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>308</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -2500,10 +2797,10 @@
     </row>
     <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B104" s="5">
-        <v>8</v>
+        <v>103</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -2511,10 +2808,10 @@
     </row>
     <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>149</v>
+        <v>310</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -2522,10 +2819,10 @@
     </row>
     <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>151</v>
+        <v>311</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -2533,10 +2830,10 @@
     </row>
     <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>153</v>
+        <v>312</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -2544,10 +2841,10 @@
     </row>
     <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>155</v>
+        <v>313</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -2555,10 +2852,10 @@
     </row>
     <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>157</v>
+        <v>314</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -2566,10 +2863,10 @@
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>159</v>
+        <v>315</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -2577,10 +2874,10 @@
     </row>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>161</v>
+        <v>316</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -2588,10 +2885,10 @@
     </row>
     <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>163</v>
+        <v>317</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -2599,10 +2896,10 @@
     </row>
     <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>165</v>
+        <v>318</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -2610,10 +2907,10 @@
     </row>
     <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B114" s="5">
-        <v>99</v>
+        <v>113</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>319</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -2621,10 +2918,10 @@
     </row>
     <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>167</v>
+        <v>114</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>168</v>
+        <v>320</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -2632,10 +2929,10 @@
     </row>
     <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>170</v>
+        <v>321</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -2643,10 +2940,10 @@
     </row>
     <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>171</v>
+        <v>116</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>172</v>
+        <v>322</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -2654,10 +2951,10 @@
     </row>
     <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>174</v>
+        <v>323</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -2665,10 +2962,10 @@
     </row>
     <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>175</v>
+        <v>118</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>176</v>
+        <v>324</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -2676,10 +2973,10 @@
     </row>
     <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>178</v>
+        <v>325</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -2687,10 +2984,10 @@
     </row>
     <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>180</v>
+        <v>326</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -2698,10 +2995,10 @@
     </row>
     <row r="122" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B122" s="5">
-        <v>84</v>
+        <v>121</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>327</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -2709,10 +3006,10 @@
     </row>
     <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B123" s="5">
-        <v>15</v>
+        <v>122</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -2720,10 +3017,10 @@
     </row>
     <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>184</v>
+        <v>329</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2731,10 +3028,10 @@
     </row>
     <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>186</v>
+        <v>330</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -2742,10 +3039,10 @@
     </row>
     <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>187</v>
+        <v>125</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>188</v>
+        <v>331</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -2753,10 +3050,10 @@
     </row>
     <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>189</v>
+        <v>126</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>190</v>
+        <v>332</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -2764,10 +3061,10 @@
     </row>
     <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>192</v>
+        <v>333</v>
       </c>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -2775,10 +3072,10 @@
     </row>
     <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>194</v>
+        <v>334</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -2786,10 +3083,10 @@
     </row>
     <row r="130" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B130" s="5">
-        <v>68</v>
+        <v>129</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>335</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -2797,10 +3094,10 @@
     </row>
     <row r="131" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B131" s="5">
-        <v>74</v>
+        <v>130</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>336</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -2808,10 +3105,10 @@
     </row>
     <row r="132" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>197</v>
+        <v>131</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>198</v>
+        <v>337</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -2819,10 +3116,10 @@
     </row>
     <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>200</v>
+        <v>338</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -2830,10 +3127,10 @@
     </row>
     <row r="134" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>201</v>
+        <v>133</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>202</v>
+        <v>339</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -2841,10 +3138,10 @@
     </row>
     <row r="135" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>203</v>
+        <v>134</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>204</v>
+        <v>340</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -2852,10 +3149,10 @@
     </row>
     <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>206</v>
+        <v>341</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -2863,10 +3160,10 @@
     </row>
     <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>208</v>
+        <v>342</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -2874,10 +3171,10 @@
     </row>
     <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B138" s="5">
-        <v>80</v>
+        <v>137</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -2885,10 +3182,10 @@
     </row>
     <row r="139" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B139" s="5">
-        <v>70</v>
+        <v>138</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>344</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -2896,10 +3193,10 @@
     </row>
     <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>211</v>
+        <v>139</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>212</v>
+        <v>345</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -2907,10 +3204,10 @@
     </row>
     <row r="141" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B141" s="5">
-        <v>78</v>
+        <v>140</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>346</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -2918,10 +3215,10 @@
     </row>
     <row r="142" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>214</v>
+        <v>141</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>215</v>
+        <v>347</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -2929,10 +3226,10 @@
     </row>
     <row r="143" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B143" s="5">
-        <v>36</v>
+        <v>142</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>348</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -2940,10 +3237,10 @@
     </row>
     <row r="144" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>217</v>
+        <v>143</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>218</v>
+        <v>349</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -2951,10 +3248,10 @@
     </row>
     <row r="145" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>219</v>
+        <v>144</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>220</v>
+        <v>350</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
@@ -2962,10 +3259,10 @@
     </row>
     <row r="146" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>221</v>
+        <v>145</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>222</v>
+        <v>351</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
@@ -2973,10 +3270,10 @@
     </row>
     <row r="147" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>223</v>
+        <v>146</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>224</v>
+        <v>352</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -2984,10 +3281,10 @@
     </row>
     <row r="148" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B148" s="5">
-        <v>64</v>
+        <v>147</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>353</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
@@ -2995,10 +3292,10 @@
     </row>
     <row r="149" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>226</v>
+        <v>148</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>227</v>
+        <v>354</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
@@ -3006,10 +3303,10 @@
     </row>
     <row r="150" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B150" s="5">
-        <v>82</v>
+        <v>149</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>355</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
@@ -3017,10 +3314,10 @@
     </row>
     <row r="151" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>229</v>
+        <v>150</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>230</v>
+        <v>356</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -3028,10 +3325,10 @@
     </row>
     <row r="152" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>231</v>
+        <v>151</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>232</v>
+        <v>357</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -3039,10 +3336,10 @@
     </row>
     <row r="153" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>233</v>
+        <v>152</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>234</v>
+        <v>358</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -3050,10 +3347,10 @@
     </row>
     <row r="154" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B154" s="5">
-        <v>89</v>
+        <v>153</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>359</v>
       </c>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -3061,10 +3358,10 @@
     </row>
     <row r="155" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B155" s="5">
-        <v>88</v>
+        <v>154</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>360</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
@@ -3072,10 +3369,10 @@
     </row>
     <row r="156" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B156" s="5">
-        <v>61</v>
+        <v>155</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>361</v>
       </c>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
@@ -3083,10 +3380,10 @@
     </row>
     <row r="157" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>238</v>
+        <v>156</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>239</v>
+        <v>362</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
@@ -3094,10 +3391,10 @@
     </row>
     <row r="158" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>240</v>
+        <v>157</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>241</v>
+        <v>363</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
@@ -3105,10 +3402,10 @@
     </row>
     <row r="159" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B159" s="5">
-        <v>50</v>
+        <v>158</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>364</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
@@ -3116,10 +3413,10 @@
     </row>
     <row r="160" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B160" s="5">
-        <v>94</v>
+        <v>159</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>365</v>
       </c>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
@@ -3127,10 +3424,10 @@
     </row>
     <row r="161" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B161" s="5">
-        <v>9</v>
+        <v>160</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>366</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
@@ -3138,10 +3435,10 @@
     </row>
     <row r="162" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>245</v>
+        <v>161</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>246</v>
+        <v>367</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -3149,10 +3446,10 @@
     </row>
     <row r="163" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B163" s="5">
-        <v>12</v>
+        <v>162</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>368</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -3160,10 +3457,10 @@
     </row>
     <row r="164" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B164" s="5">
-        <v>13</v>
+        <v>163</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>369</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -3171,10 +3468,10 @@
     </row>
     <row r="165" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B165" s="5">
-        <v>14</v>
+        <v>164</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>370</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
@@ -3182,10 +3479,10 @@
     </row>
     <row r="166" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>251</v>
+        <v>371</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
@@ -3193,10 +3490,10 @@
     </row>
     <row r="167" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B167" s="5">
-        <v>16</v>
+        <v>166</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>372</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -3204,10 +3501,10 @@
     </row>
     <row r="168" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
-        <v>253</v>
+        <v>167</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>254</v>
+        <v>373</v>
       </c>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -3215,10 +3512,10 @@
     </row>
     <row r="169" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
-        <v>255</v>
+        <v>168</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>256</v>
+        <v>374</v>
       </c>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -3226,10 +3523,10 @@
     </row>
     <row r="170" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B170" s="5">
-        <v>20</v>
+        <v>169</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>375</v>
       </c>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
@@ -3237,10 +3534,10 @@
     </row>
     <row r="171" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B171" s="5">
-        <v>21</v>
+        <v>170</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>376</v>
       </c>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
@@ -3248,10 +3545,10 @@
     </row>
     <row r="172" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B172" s="5">
-        <v>69</v>
+        <v>171</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>377</v>
       </c>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
@@ -3259,10 +3556,10 @@
     </row>
     <row r="173" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B173" s="5">
-        <v>75</v>
+        <v>172</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>378</v>
       </c>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
@@ -3270,10 +3567,10 @@
     </row>
     <row r="174" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>261</v>
+        <v>173</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>262</v>
+        <v>379</v>
       </c>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
@@ -3281,10 +3578,10 @@
     </row>
     <row r="175" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B175" s="5">
-        <v>81</v>
+        <v>174</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>380</v>
       </c>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
@@ -3292,10 +3589,10 @@
     </row>
     <row r="176" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B176" s="5">
-        <v>71</v>
+        <v>175</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>381</v>
       </c>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -3303,10 +3600,10 @@
     </row>
     <row r="177" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>265</v>
+        <v>176</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>266</v>
+        <v>382</v>
       </c>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -3314,10 +3611,10 @@
     </row>
     <row r="178" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B178" s="5">
-        <v>79</v>
+        <v>177</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>383</v>
       </c>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -3325,10 +3622,10 @@
     </row>
     <row r="179" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>268</v>
+        <v>178</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>269</v>
+        <v>384</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -3336,10 +3633,10 @@
     </row>
     <row r="180" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B180" s="5">
-        <v>37</v>
+        <v>179</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -3347,10 +3644,10 @@
     </row>
     <row r="181" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>271</v>
+        <v>180</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>272</v>
+        <v>386</v>
       </c>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
@@ -3358,10 +3655,10 @@
     </row>
     <row r="182" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B182" s="5">
-        <v>40</v>
+        <v>181</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>387</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
@@ -3369,10 +3666,10 @@
     </row>
     <row r="183" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B183" s="5">
-        <v>41</v>
+        <v>182</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>388</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
@@ -3380,10 +3677,10 @@
     </row>
     <row r="184" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B184" s="5">
-        <v>42</v>
+        <v>183</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>389</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
@@ -3391,10 +3688,10 @@
     </row>
     <row r="185" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B185" s="5">
-        <v>65</v>
+        <v>184</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>390</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
@@ -3402,10 +3699,10 @@
     </row>
     <row r="186" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>277</v>
+        <v>185</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>278</v>
+        <v>391</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
@@ -3413,10 +3710,10 @@
     </row>
     <row r="187" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B187" s="5">
-        <v>83</v>
+        <v>186</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>392</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
@@ -3424,10 +3721,10 @@
     </row>
     <row r="188" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>280</v>
+        <v>187</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>281</v>
+        <v>393</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
@@ -3435,10 +3732,10 @@
     </row>
     <row r="189" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>282</v>
+        <v>188</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>283</v>
+        <v>394</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
@@ -3446,10 +3743,10 @@
     </row>
     <row r="190" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>284</v>
+        <v>189</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>285</v>
+        <v>395</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
@@ -3457,10 +3754,10 @@
     </row>
     <row r="191" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>286</v>
+        <v>190</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>287</v>
+        <v>396</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
@@ -3468,10 +3765,10 @@
     </row>
     <row r="192" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>288</v>
+        <v>191</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>289</v>
+        <v>397</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
@@ -3479,10 +3776,10 @@
     </row>
     <row r="193" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B193" s="5">
-        <v>0</v>
+        <v>192</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>398</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
@@ -3490,10 +3787,10 @@
     </row>
     <row r="194" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B194" s="5">
-        <v>57</v>
+        <v>193</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>399</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
@@ -3501,10 +3798,10 @@
     </row>
     <row r="195" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B195" s="5">
-        <v>58</v>
+        <v>194</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>400</v>
       </c>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
@@ -3512,10 +3809,10 @@
     </row>
     <row r="196" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>293</v>
+        <v>195</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>294</v>
+        <v>401</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
@@ -3523,10 +3820,10 @@
     </row>
     <row r="197" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>295</v>
+        <v>196</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>296</v>
+        <v>402</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -3534,10 +3831,10 @@
     </row>
     <row r="198" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>297</v>
+        <v>197</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>298</v>
+        <v>403</v>
       </c>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
@@ -3545,10 +3842,10 @@
     </row>
     <row r="199" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>299</v>
+        <v>198</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>300</v>
+        <v>404</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
@@ -3556,10 +3853,10 @@
     </row>
     <row r="200" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B200" s="5">
-        <v>35</v>
+        <v>199</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>405</v>
       </c>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
@@ -3567,10 +3864,10 @@
     </row>
     <row r="201" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B201" s="5">
-        <v>56</v>
+        <v>200</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>406</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -3578,10 +3875,10 @@
     </row>
     <row r="202" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B202" s="5">
-        <v>11</v>
+        <v>201</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>407</v>
       </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
@@ -3589,10 +3886,10 @@
     </row>
     <row r="203" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>304</v>
+        <v>202</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>305</v>
+        <v>408</v>
       </c>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -3600,10 +3897,10 @@
     </row>
     <row r="204" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>306</v>
+        <v>203</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>307</v>
+        <v>409</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -3611,10 +3908,10 @@
     </row>
     <row r="205" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="s">
-        <v>308</v>
+        <v>204</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>309</v>
+        <v>410</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
@@ -3622,11 +3919,9 @@
     </row>
     <row r="206" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="B206" s="5" t="s">
-        <v>311</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B206" s="5"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>

</xml_diff>

<commit_message>
Push opcodes & opcode sequences upstream, written code for vulnerability classification
Signed-off-by: JayJay <jwanjohi95@gmail.com>
</commit_message>
<xml_diff>
--- a/Java_Bytecode_Instructions.xlsx
+++ b/Java_Bytecode_Instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="320">
   <si>
     <t>aaload</t>
   </si>
@@ -641,9 +641,6 @@
     <t>wide</t>
   </si>
   <si>
-    <t>(no name)</t>
-  </si>
-  <si>
     <t>2a</t>
   </si>
   <si>
@@ -959,7 +956,34 @@
     <t>c4</t>
   </si>
   <si>
-    <t>cb-fd</t>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -997,11 +1021,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1285,21 +1309,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="E207" sqref="E207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>32</v>
       </c>
     </row>
@@ -1307,7 +1331,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>53</v>
       </c>
     </row>
@@ -1315,15 +1339,15 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>19</v>
       </c>
     </row>
@@ -1331,111 +1355,111 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>206</v>
+      <c r="B5" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>207</v>
+      <c r="B6" s="1" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>208</v>
+      <c r="B7" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>209</v>
+      <c r="B8" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>210</v>
+      <c r="B9" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>211</v>
+      <c r="B10" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>212</v>
+      <c r="B11" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>213</v>
+      <c r="B12" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>214</v>
+      <c r="B13" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>215</v>
+      <c r="B14" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>216</v>
+      <c r="B15" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>217</v>
+      <c r="B16" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>218</v>
+      <c r="B17" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>33</v>
       </c>
     </row>
@@ -1443,7 +1467,7 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>54</v>
       </c>
     </row>
@@ -1451,7 +1475,7 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1459,15 +1483,15 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>219</v>
+      <c r="B21" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>34</v>
       </c>
     </row>
@@ -1475,7 +1499,7 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>55</v>
       </c>
     </row>
@@ -1483,15 +1507,15 @@
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>220</v>
+      <c r="B24" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>90</v>
       </c>
     </row>
@@ -1499,23 +1523,23 @@
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>221</v>
+      <c r="B26" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>222</v>
+      <c r="B27" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>63</v>
       </c>
     </row>
@@ -1523,7 +1547,7 @@
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>31</v>
       </c>
     </row>
@@ -1531,7 +1555,7 @@
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>52</v>
       </c>
     </row>
@@ -1539,7 +1563,7 @@
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>98</v>
       </c>
     </row>
@@ -1547,7 +1571,7 @@
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>97</v>
       </c>
     </row>
@@ -1555,31 +1579,31 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>223</v>
+      <c r="B33" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>224</v>
+      <c r="B34" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>225</v>
+      <c r="B35" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>18</v>
       </c>
     </row>
@@ -1587,7 +1611,7 @@
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>26</v>
       </c>
     </row>
@@ -1595,7 +1619,7 @@
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>27</v>
       </c>
     </row>
@@ -1603,7 +1627,7 @@
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>28</v>
       </c>
     </row>
@@ -1611,7 +1635,7 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>29</v>
       </c>
     </row>
@@ -1619,15 +1643,15 @@
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>226</v>
+      <c r="B41" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>77</v>
       </c>
     </row>
@@ -1635,7 +1659,7 @@
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>73</v>
       </c>
     </row>
@@ -1643,15 +1667,15 @@
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>227</v>
+      <c r="B44" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>39</v>
       </c>
     </row>
@@ -1659,7 +1683,7 @@
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>47</v>
       </c>
     </row>
@@ -1667,7 +1691,7 @@
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>48</v>
       </c>
     </row>
@@ -1675,7 +1699,7 @@
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>49</v>
       </c>
     </row>
@@ -1683,15 +1707,15 @@
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>228</v>
+      <c r="B49" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>67</v>
       </c>
     </row>
@@ -1699,7 +1723,7 @@
       <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>59</v>
       </c>
     </row>
@@ -1707,71 +1731,71 @@
       <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>229</v>
+      <c r="B52" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>230</v>
+      <c r="B53" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>231</v>
+      <c r="B54" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>232</v>
+      <c r="B55" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>233</v>
+      <c r="B56" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>234</v>
+      <c r="B57" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>235</v>
+      <c r="B58" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>236</v>
+      <c r="B59" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>62</v>
       </c>
     </row>
@@ -1779,7 +1803,7 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>30</v>
       </c>
     </row>
@@ -1787,7 +1811,7 @@
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>51</v>
       </c>
     </row>
@@ -1795,7 +1819,7 @@
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>96</v>
       </c>
     </row>
@@ -1803,7 +1827,7 @@
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>95</v>
       </c>
     </row>
@@ -1811,39 +1835,39 @@
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>237</v>
+      <c r="B65" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>238</v>
+      <c r="B66" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>239</v>
+      <c r="B67" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>240</v>
+      <c r="B68" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>17</v>
       </c>
     </row>
@@ -1851,7 +1875,7 @@
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>22</v>
       </c>
     </row>
@@ -1859,7 +1883,7 @@
       <c r="A71" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>23</v>
       </c>
     </row>
@@ -1867,7 +1891,7 @@
       <c r="A72" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>24</v>
       </c>
     </row>
@@ -1875,7 +1899,7 @@
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>25</v>
       </c>
     </row>
@@ -1883,15 +1907,15 @@
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>241</v>
+      <c r="B74" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>76</v>
       </c>
     </row>
@@ -1899,7 +1923,7 @@
       <c r="A76" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>72</v>
       </c>
     </row>
@@ -1907,15 +1931,15 @@
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>242</v>
+      <c r="B77" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>38</v>
       </c>
     </row>
@@ -1923,7 +1947,7 @@
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>43</v>
       </c>
     </row>
@@ -1931,7 +1955,7 @@
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>44</v>
       </c>
     </row>
@@ -1939,7 +1963,7 @@
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>45</v>
       </c>
     </row>
@@ -1947,7 +1971,7 @@
       <c r="A82" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>46</v>
       </c>
     </row>
@@ -1955,7 +1979,7 @@
       <c r="A83" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>66</v>
       </c>
     </row>
@@ -1963,39 +1987,39 @@
       <c r="A84" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>243</v>
+      <c r="B84" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>244</v>
+      <c r="B85" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>245</v>
+      <c r="B86" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>246</v>
+      <c r="B87" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>91</v>
       </c>
     </row>
@@ -2003,7 +2027,7 @@
       <c r="A89" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>92</v>
       </c>
     </row>
@@ -2011,7 +2035,7 @@
       <c r="A90" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>87</v>
       </c>
     </row>
@@ -2019,7 +2043,7 @@
       <c r="A91" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>86</v>
       </c>
     </row>
@@ -2027,7 +2051,7 @@
       <c r="A92" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>85</v>
       </c>
     </row>
@@ -2035,7 +2059,7 @@
       <c r="A93" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>93</v>
       </c>
     </row>
@@ -2043,7 +2067,7 @@
       <c r="A94" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>60</v>
       </c>
     </row>
@@ -2051,159 +2075,159 @@
       <c r="A95" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>247</v>
+      <c r="B95" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>248</v>
+      <c r="B96" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>249</v>
+      <c r="B97" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="2">
-        <v>2</v>
+      <c r="B98" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="2">
-        <v>3</v>
+      <c r="B99" s="1" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="2">
-        <v>4</v>
+      <c r="B100" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="2">
-        <v>5</v>
+      <c r="B101" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="2">
-        <v>6</v>
+      <c r="B102" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="2">
-        <v>7</v>
+      <c r="B103" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="2">
-        <v>8</v>
+      <c r="B104" s="1" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>250</v>
+      <c r="B105" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>251</v>
+      <c r="B106" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>252</v>
+      <c r="B107" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>253</v>
+      <c r="B108" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>254</v>
+      <c r="B109" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>255</v>
+      <c r="B110" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>256</v>
+      <c r="B111" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>257</v>
+      <c r="B112" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>258</v>
+      <c r="B113" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114" s="1">
         <v>99</v>
       </c>
     </row>
@@ -2211,63 +2235,63 @@
       <c r="A115" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>259</v>
+      <c r="B115" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>260</v>
+      <c r="B116" s="1" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>261</v>
+      <c r="B117" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>262</v>
+      <c r="B118" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>263</v>
+      <c r="B119" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>264</v>
+      <c r="B120" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>265</v>
+      <c r="B121" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122" s="1">
         <v>84</v>
       </c>
     </row>
@@ -2275,7 +2299,7 @@
       <c r="A123" t="s">
         <v>122</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123" s="1">
         <v>15</v>
       </c>
     </row>
@@ -2283,55 +2307,55 @@
       <c r="A124" t="s">
         <v>123</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>266</v>
+      <c r="B124" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-      <c r="B125" s="2" t="s">
-        <v>267</v>
+      <c r="B125" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>268</v>
+      <c r="B126" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>269</v>
+      <c r="B127" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>270</v>
+      <c r="B128" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>271</v>
+      <c r="B129" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130" s="1">
         <v>68</v>
       </c>
     </row>
@@ -2339,7 +2363,7 @@
       <c r="A131" t="s">
         <v>130</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131" s="1">
         <v>74</v>
       </c>
     </row>
@@ -2347,55 +2371,55 @@
       <c r="A132" t="s">
         <v>131</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>272</v>
+      <c r="B132" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>273</v>
+      <c r="B133" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>274</v>
+      <c r="B134" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>275</v>
+      <c r="B135" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>276</v>
+      <c r="B136" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>277</v>
+      <c r="B137" s="1" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B138" s="1">
         <v>80</v>
       </c>
     </row>
@@ -2403,7 +2427,7 @@
       <c r="A139" t="s">
         <v>138</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B139" s="1">
         <v>70</v>
       </c>
     </row>
@@ -2411,15 +2435,15 @@
       <c r="A140" t="s">
         <v>139</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>278</v>
+      <c r="B140" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B141" s="1">
         <v>78</v>
       </c>
     </row>
@@ -2427,15 +2451,15 @@
       <c r="A142" t="s">
         <v>141</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>279</v>
+      <c r="B142" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B143" s="1">
         <v>36</v>
       </c>
     </row>
@@ -2443,39 +2467,39 @@
       <c r="A144" t="s">
         <v>143</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>280</v>
+      <c r="B144" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>281</v>
+      <c r="B145" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>282</v>
+      <c r="B146" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>283</v>
+      <c r="B147" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="1">
         <v>64</v>
       </c>
     </row>
@@ -2483,15 +2507,15 @@
       <c r="A149" t="s">
         <v>148</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>284</v>
+      <c r="B149" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150" s="1">
         <v>82</v>
       </c>
     </row>
@@ -2499,31 +2523,31 @@
       <c r="A151" t="s">
         <v>150</v>
       </c>
-      <c r="B151" s="2" t="s">
-        <v>285</v>
+      <c r="B151" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-      <c r="B152" s="2" t="s">
-        <v>286</v>
+      <c r="B152" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>287</v>
+      <c r="B153" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B154" s="1">
         <v>89</v>
       </c>
     </row>
@@ -2531,7 +2555,7 @@
       <c r="A155" t="s">
         <v>154</v>
       </c>
-      <c r="B155" s="2">
+      <c r="B155" s="1">
         <v>88</v>
       </c>
     </row>
@@ -2539,7 +2563,7 @@
       <c r="A156" t="s">
         <v>155</v>
       </c>
-      <c r="B156" s="2">
+      <c r="B156" s="1">
         <v>61</v>
       </c>
     </row>
@@ -2547,23 +2571,23 @@
       <c r="A157" t="s">
         <v>156</v>
       </c>
-      <c r="B157" s="2" t="s">
-        <v>288</v>
+      <c r="B157" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-      <c r="B158" s="2" t="s">
-        <v>289</v>
+      <c r="B158" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B159" s="1">
         <v>50</v>
       </c>
     </row>
@@ -2571,7 +2595,7 @@
       <c r="A160" t="s">
         <v>159</v>
       </c>
-      <c r="B160" s="2">
+      <c r="B160" s="1">
         <v>94</v>
       </c>
     </row>
@@ -2579,23 +2603,23 @@
       <c r="A161" t="s">
         <v>160</v>
       </c>
-      <c r="B161" s="2">
-        <v>9</v>
+      <c r="B161" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>290</v>
+      <c r="B162" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-      <c r="B163" s="2">
+      <c r="B163" s="1">
         <v>12</v>
       </c>
     </row>
@@ -2603,7 +2627,7 @@
       <c r="A164" t="s">
         <v>163</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B164" s="1">
         <v>13</v>
       </c>
     </row>
@@ -2611,7 +2635,7 @@
       <c r="A165" t="s">
         <v>164</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B165" s="1">
         <v>14</v>
       </c>
     </row>
@@ -2619,15 +2643,15 @@
       <c r="A166" t="s">
         <v>165</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>291</v>
+      <c r="B166" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B167" s="1">
         <v>16</v>
       </c>
     </row>
@@ -2635,23 +2659,23 @@
       <c r="A168" t="s">
         <v>167</v>
       </c>
-      <c r="B168" s="2" t="s">
-        <v>292</v>
+      <c r="B168" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-      <c r="B169" s="2" t="s">
-        <v>293</v>
+      <c r="B169" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B170" s="1">
         <v>20</v>
       </c>
     </row>
@@ -2659,7 +2683,7 @@
       <c r="A171" t="s">
         <v>170</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B171" s="1">
         <v>21</v>
       </c>
     </row>
@@ -2667,7 +2691,7 @@
       <c r="A172" t="s">
         <v>171</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B172" s="1">
         <v>69</v>
       </c>
     </row>
@@ -2675,7 +2699,7 @@
       <c r="A173" t="s">
         <v>172</v>
       </c>
-      <c r="B173" s="2">
+      <c r="B173" s="1">
         <v>75</v>
       </c>
     </row>
@@ -2683,15 +2707,15 @@
       <c r="A174" t="s">
         <v>173</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>294</v>
+      <c r="B174" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-      <c r="B175" s="2">
+      <c r="B175" s="1">
         <v>81</v>
       </c>
     </row>
@@ -2699,7 +2723,7 @@
       <c r="A176" t="s">
         <v>175</v>
       </c>
-      <c r="B176" s="2">
+      <c r="B176" s="1">
         <v>71</v>
       </c>
     </row>
@@ -2707,15 +2731,15 @@
       <c r="A177" t="s">
         <v>176</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>295</v>
+      <c r="B177" s="1" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B178" s="1">
         <v>79</v>
       </c>
     </row>
@@ -2723,15 +2747,15 @@
       <c r="A179" t="s">
         <v>178</v>
       </c>
-      <c r="B179" s="2" t="s">
-        <v>296</v>
+      <c r="B179" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B180" s="1">
         <v>37</v>
       </c>
     </row>
@@ -2739,15 +2763,15 @@
       <c r="A181" t="s">
         <v>180</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>297</v>
+      <c r="B181" s="1" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182" s="1">
         <v>40</v>
       </c>
     </row>
@@ -2755,7 +2779,7 @@
       <c r="A183" t="s">
         <v>182</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183" s="1">
         <v>41</v>
       </c>
     </row>
@@ -2763,7 +2787,7 @@
       <c r="A184" t="s">
         <v>183</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="1">
         <v>42</v>
       </c>
     </row>
@@ -2771,7 +2795,7 @@
       <c r="A185" t="s">
         <v>184</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185" s="1">
         <v>65</v>
       </c>
     </row>
@@ -2779,15 +2803,15 @@
       <c r="A186" t="s">
         <v>185</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>298</v>
+      <c r="B186" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
-      <c r="B187" s="2">
+      <c r="B187" s="1">
         <v>83</v>
       </c>
     </row>
@@ -2795,55 +2819,55 @@
       <c r="A188" t="s">
         <v>187</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>299</v>
+      <c r="B188" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>300</v>
+      <c r="B189" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>301</v>
+      <c r="B190" s="1" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>302</v>
+      <c r="B191" s="1" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>303</v>
+      <c r="B192" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-      <c r="B193" s="2">
-        <v>0</v>
+      <c r="B193" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-      <c r="B194" s="2">
+      <c r="B194" s="1">
         <v>57</v>
       </c>
     </row>
@@ -2851,7 +2875,7 @@
       <c r="A195" t="s">
         <v>194</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B195" s="1">
         <v>58</v>
       </c>
     </row>
@@ -2859,39 +2883,39 @@
       <c r="A196" t="s">
         <v>195</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>304</v>
+      <c r="B196" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-      <c r="B197" s="2" t="s">
-        <v>305</v>
+      <c r="B197" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>306</v>
+      <c r="B198" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-      <c r="B199" s="2" t="s">
-        <v>307</v>
+      <c r="B199" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-      <c r="B200" s="2">
+      <c r="B200" s="1">
         <v>35</v>
       </c>
     </row>
@@ -2899,7 +2923,7 @@
       <c r="A201" t="s">
         <v>200</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B201" s="1">
         <v>56</v>
       </c>
     </row>
@@ -2907,7 +2931,7 @@
       <c r="A202" t="s">
         <v>201</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B202" s="1">
         <v>11</v>
       </c>
     </row>
@@ -2915,39 +2939,34 @@
       <c r="A203" t="s">
         <v>202</v>
       </c>
-      <c r="B203" s="2" t="s">
-        <v>308</v>
+      <c r="B203" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>309</v>
+      <c r="B204" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>310</v>
+      <c r="B205" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>205</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>311</v>
-      </c>
+      <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B207" s="2"/>
+      <c r="B207" s="1"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B208" s="2"/>
+      <c r="B208" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>